<commit_message>
updated template file & fixed bulk upload
</commit_message>
<xml_diff>
--- a/src/main/resources/Items.xlsx
+++ b/src/main/resources/Items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Archit Maniyath\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Archit Maniyath\resume_projects\springboot\expense-tracker-api\tenant-system-api\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F59E6C4-309C-4567-ADEE-98162E4E7C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833A08D3-F708-415B-9465-DE9847CCB42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42BEA93D-9A8D-4B48-9A54-F255004BAC14}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>itemname</t>
   </si>
@@ -59,21 +59,6 @@
     <t>tesco</t>
   </si>
   <si>
-    <t>20-02-2022</t>
-  </si>
-  <si>
-    <t>20-03-2022</t>
-  </si>
-  <si>
-    <t>20-04-2022</t>
-  </si>
-  <si>
-    <t>20-05-2022</t>
-  </si>
-  <si>
-    <t>20-06-2022</t>
-  </si>
-  <si>
     <t>Lidl</t>
   </si>
   <si>
@@ -87,6 +72,9 @@
   </si>
   <si>
     <t>Bread</t>
+  </si>
+  <si>
+    <t>2022-10-20</t>
   </si>
 </sst>
 </file>
@@ -442,7 +430,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,15 +469,15 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -498,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -506,7 +494,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -515,15 +503,15 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -532,12 +520,12 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -549,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>